<commit_message>
remove figures, tables, xlsx
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -35,7 +35,54 @@
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">Random programs: A+GCS preferred to B</t>
+    <t xml:space="preserve">Global climate scheme (GCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National tax on millionaires funding public services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global tax on millionaires funding low-income countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred share of global wealth
+tax for low-income countries: ≥ 30%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Country]'s foreign aid should be increased*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-income countries contributing $100 billion per year
+to help low-income countries adapt to climate change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-income countries funding renewable
+energy in low-income countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payments from high-income countries to compensate
+low-income countries for climate damages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation of low-income countries' public debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratise international institutions (UN, IMF) by making
+a country's voting right proportional to its population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removing tariffs on imports from low-income countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A minimum wage in all countries
+at 50% of local median wage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fight tax evasion by creating a global financial
+register to record ownership of all assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A maximum wealth limit of $10 billion
+(US) / €100 million (Eu) for each human</t>
   </si>
 </sst>
 </file>
@@ -395,22 +442,321 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.590432228283676</v>
+        <v>0.542040004729187</v>
       </c>
       <c r="C2" t="n">
-        <v>0.601344860710855</v>
+        <v>0.757320866764204</v>
       </c>
       <c r="D2" t="n">
-        <v>0.613245033112583</v>
+        <v>0.802845995450502</v>
       </c>
       <c r="E2" t="n">
-        <v>0.587147030185005</v>
+        <v>0.712681465751731</v>
       </c>
       <c r="F2" t="n">
-        <v>0.640070921985816</v>
+        <v>0.809917713113721</v>
       </c>
       <c r="G2" t="n">
-        <v>0.58043758043758</v>
+        <v>0.74106127773703</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.619576204293734</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.758375208534753</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.697490019207693</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.785605734377313</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.788109233298969</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.774030617727549</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.580974048697037</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.714793319488843</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.694319177328758</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.723244532725875</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.776824002261202</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.708989998773392</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.502686637940573</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.535405079823794</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.53495530999455</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.504405401186565</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.57374820373221</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.54094700051697</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.598187005678365</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.636739028674537</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.627588384954585</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.676807601959896</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.691059073949057</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.560844998477962</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.45011340420921</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.580303842050924</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.554844714670846</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.597860385545241</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.624386789670735</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.54091224731223</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.53081419263325</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.646086050975591</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.617631776703308</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.661981009518735</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.679241918379181</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.624160044931323</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.409115346811486</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.535873014459192</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.522108726136302</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.528761543405907</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.619349694288149</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.510164860189199</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.308391076954102</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.365731640324952</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.362994387715357</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.298641910128985</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.450925576392201</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.404799933538172</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.3441053797594</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.443594773467438</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.436219325369461</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.428402025624624</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.517519698549576</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.432189204736391</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.390484602228333</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.49094991581821</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.386302468418039</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.512592712201629</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.502893401333253</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.540728143603005</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.41536013985638</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.547947048183082</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.541679032092289</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.542087544034292</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.60768384976524</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.531644320070783</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.441485472151688</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.699336514515305</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.730152208937297</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.702462385725501</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.718628182752579</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.6490870831924</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.335948876827959</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.45314379468064</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.395498925733041</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.479942664267705</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.441371326747748</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.496306674811346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>